<commit_message>
reformatted file_refactor to use set comprehension
</commit_message>
<xml_diff>
--- a/test/test_data.xlsx
+++ b/test/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1mike\PycharmProjects\libRL package\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B68CEB8-42DC-431E-A9BE-1035E170E824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0992F7AE-5B68-4779-8CE8-2F51315CF16F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50FF7A3F-1390-47A9-BDA6-0EA563ADF9B3}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>